<commit_message>
Package 15 release candidate
</commit_message>
<xml_diff>
--- a/curation/draft/crf/CRF_MH.xlsx
+++ b/curation/draft/crf/CRF_MH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\crf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD84CFF-490C-474F-BA3E-AD05C0368E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF10CCA7-C7AA-489B-A594-01E6D88AA558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRF_MH" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>MHCAT</t>
   </si>
   <si>
-    <t>C83018</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -266,18 +263,9 @@
     <t>MHOCCUR</t>
   </si>
   <si>
-    <t>C87897</t>
-  </si>
-  <si>
-    <t>C83067</t>
-  </si>
-  <si>
     <t>MHSCAT</t>
   </si>
   <si>
-    <t>C83143</t>
-  </si>
-  <si>
     <t>Medical History Category</t>
   </si>
   <si>
@@ -408,6 +396,18 @@
   </si>
   <si>
     <t>completion_instructions</t>
+  </si>
+  <si>
+    <t>C25692</t>
+  </si>
+  <si>
+    <t>C25372</t>
+  </si>
+  <si>
+    <t>C127786</t>
+  </si>
+  <si>
+    <t>C171000</t>
   </si>
 </sst>
 </file>
@@ -806,10 +806,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="112" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U1" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
@@ -870,13 +870,13 @@
         <v>8</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -891,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>14</v>
@@ -912,10 +912,10 @@
         <v>19</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>20</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
@@ -968,7 +968,7 @@
         <v>32</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M2" t="s">
         <v>33</v>
@@ -977,7 +977,7 @@
         <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P2" t="s">
         <v>34</v>
@@ -995,10 +995,10 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>35</v>
@@ -1007,21 +1007,21 @@
         <v>36</v>
       </c>
       <c r="AE2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -1030,7 +1030,7 @@
         <v>32</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M3" t="s">
         <v>37</v>
@@ -1039,19 +1039,19 @@
         <v>37</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S3">
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V3">
         <v>10</v>
@@ -1077,19 +1077,19 @@
         <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M4" t="s">
         <v>50</v>
@@ -1098,16 +1098,16 @@
         <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S4">
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U4" t="s">
         <v>44</v>
@@ -1119,13 +1119,13 @@
         <v>43</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AH4" t="s">
         <v>50</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -1139,37 +1139,37 @@
         <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O5" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S5">
         <v>2</v>
       </c>
       <c r="T5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U5" t="s">
         <v>44</v>
@@ -1181,15 +1181,15 @@
         <v>43</v>
       </c>
       <c r="AH5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -1198,46 +1198,46 @@
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="S6">
         <v>3</v>
       </c>
       <c r="T6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V6">
         <v>2</v>
       </c>
       <c r="AH6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -1251,19 +1251,19 @@
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M7" t="s">
         <v>41</v>
@@ -1275,7 +1275,7 @@
         <v>42</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S7">
         <v>4</v>
@@ -1307,19 +1307,19 @@
         <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M8" t="s">
         <v>45</v>
@@ -1328,19 +1328,19 @@
         <v>45</v>
       </c>
       <c r="O8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S8">
         <v>5</v>
       </c>
       <c r="T8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V8">
         <v>10</v>
@@ -1363,35 +1363,35 @@
         <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U9" t="s">
         <v>44</v>
@@ -1400,10 +1400,10 @@
         <v>1</v>
       </c>
       <c r="AA9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB9" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB9" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>35</v>
@@ -1412,13 +1412,13 @@
         <v>36</v>
       </c>
       <c r="AE9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -1432,19 +1432,19 @@
         <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M10" t="s">
         <v>48</v>
@@ -1453,19 +1453,19 @@
         <v>48</v>
       </c>
       <c r="O10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S10">
         <v>7</v>
       </c>
       <c r="T10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V10">
         <v>10</v>
@@ -1488,19 +1488,19 @@
         <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G11" t="s">
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M11" t="s">
         <v>47</v>
@@ -1509,16 +1509,16 @@
         <v>47</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S11">
         <v>8</v>
       </c>
       <c r="T11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U11" t="s">
         <v>44</v>
@@ -1527,10 +1527,10 @@
         <v>1</v>
       </c>
       <c r="AA11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB11" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB11" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>35</v>
@@ -1539,13 +1539,13 @@
         <v>36</v>
       </c>
       <c r="AE11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="60" x14ac:dyDescent="0.25">
@@ -1553,25 +1553,25 @@
         <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I12" t="s">
+        <v>104</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="M12" t="s">
         <v>50</v>
@@ -1580,16 +1580,16 @@
         <v>50</v>
       </c>
       <c r="O12" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S12">
         <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U12" t="s">
         <v>44</v>
@@ -1601,13 +1601,13 @@
         <v>43</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="AH12" t="s">
         <v>50</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -1615,43 +1615,43 @@
         <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>112</v>
-      </c>
       <c r="M13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O13" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S13">
         <v>2</v>
       </c>
       <c r="T13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U13" t="s">
         <v>44</v>
@@ -1663,10 +1663,10 @@
         <v>43</v>
       </c>
       <c r="AH13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -1674,25 +1674,25 @@
         <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="M14" t="s">
         <v>41</v>
@@ -1704,7 +1704,7 @@
         <v>42</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S14">
         <v>3</v>
@@ -1730,37 +1730,37 @@
         <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>112</v>
-      </c>
       <c r="M15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O15" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S15">
         <v>4</v>
@@ -1778,10 +1778,10 @@
         <v>43</v>
       </c>
       <c r="AA15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB15" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB15" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
@@ -1789,13 +1789,13 @@
         <v>43</v>
       </c>
       <c r="AG15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AH15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="45" x14ac:dyDescent="0.25">
@@ -1803,37 +1803,37 @@
         <v>39</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>112</v>
-      </c>
       <c r="M16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O16" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S16">
         <v>5</v>
@@ -1848,10 +1848,10 @@
         <v>1</v>
       </c>
       <c r="AA16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB16" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB16" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC16" s="1" t="s">
         <v>35</v>
@@ -1860,13 +1860,13 @@
         <v>36</v>
       </c>
       <c r="AE16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="30" x14ac:dyDescent="0.25">
@@ -1874,25 +1874,25 @@
         <v>39</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I17" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="M17" t="s">
         <v>45</v>
@@ -1901,10 +1901,10 @@
         <v>45</v>
       </c>
       <c r="O17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S17">
         <v>6</v>
@@ -1913,7 +1913,7 @@
         <v>43</v>
       </c>
       <c r="U17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V17">
         <v>10</v>
@@ -1930,25 +1930,25 @@
         <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I18" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="M18" t="s">
         <v>48</v>
@@ -1957,19 +1957,19 @@
         <v>48</v>
       </c>
       <c r="O18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S18">
         <v>7</v>
       </c>
       <c r="T18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V18">
         <v>10</v>
@@ -1986,25 +1986,25 @@
         <v>39</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="M19" t="s">
         <v>47</v>
@@ -2013,16 +2013,16 @@
         <v>47</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S19">
         <v>8</v>
       </c>
       <c r="T19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U19" t="s">
         <v>44</v>
@@ -2031,10 +2031,10 @@
         <v>1</v>
       </c>
       <c r="AA19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB19" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB19" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC19" s="1" t="s">
         <v>35</v>
@@ -2043,13 +2043,13 @@
         <v>36</v>
       </c>
       <c r="AE19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:35" ht="45" x14ac:dyDescent="0.25">
@@ -2057,28 +2057,28 @@
         <v>39</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
       </c>
       <c r="H20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K20" s="2">
         <v>360</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M20" t="s">
         <v>41</v>
@@ -2090,7 +2090,7 @@
         <v>42</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -2105,13 +2105,13 @@
         <v>200</v>
       </c>
       <c r="AF20" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AH20" t="s">
         <v>41</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:35" ht="45" x14ac:dyDescent="0.25">
@@ -2119,40 +2119,40 @@
         <v>39</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K21" s="2">
         <v>360</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O21" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S21">
         <v>2</v>
@@ -2170,10 +2170,10 @@
         <v>43</v>
       </c>
       <c r="AA21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB21" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB21" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
@@ -2181,13 +2181,13 @@
         <v>43</v>
       </c>
       <c r="AG21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AH21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:35" ht="45" x14ac:dyDescent="0.25">
@@ -2195,46 +2195,46 @@
         <v>39</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G22" t="s">
         <v>32</v>
       </c>
       <c r="H22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K22" s="2">
         <v>360</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O22" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="S22">
         <v>3</v>
       </c>
       <c r="T22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U22" t="s">
         <v>44</v>
@@ -2246,10 +2246,10 @@
         <v>43</v>
       </c>
       <c r="AA22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB22" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB22" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -2257,13 +2257,13 @@
         <v>43</v>
       </c>
       <c r="AG22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AH22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:35" ht="45" x14ac:dyDescent="0.25">
@@ -2271,37 +2271,37 @@
         <v>39</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G23" t="s">
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K23" s="2">
         <v>360</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S23">
         <v>4</v>
@@ -2319,24 +2319,24 @@
         <v>43</v>
       </c>
       <c r="AA23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AF23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AG23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:35" ht="45" x14ac:dyDescent="0.25">
@@ -2344,28 +2344,28 @@
         <v>39</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G24" t="s">
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K24" s="2">
         <v>360</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M24" t="s">
         <v>45</v>
@@ -2374,10 +2374,10 @@
         <v>45</v>
       </c>
       <c r="O24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="S24">
         <v>5</v>
@@ -2386,7 +2386,7 @@
         <v>43</v>
       </c>
       <c r="U24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V24">
         <v>10</v>
@@ -2403,28 +2403,28 @@
         <v>39</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K25" s="2">
         <v>360</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M25" t="s">
         <v>47</v>
@@ -2433,16 +2433,16 @@
         <v>47</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S25">
         <v>6</v>
       </c>
       <c r="T25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U25" t="s">
         <v>44</v>
@@ -2454,10 +2454,10 @@
         <v>43</v>
       </c>
       <c r="AA25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB25" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="AB25" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
@@ -2465,13 +2465,13 @@
         <v>43</v>
       </c>
       <c r="AG25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="AH25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>